<commit_message>
All Classifiers Validation Performance
</commit_message>
<xml_diff>
--- a/A1_Experiment_Sheet.xlsx
+++ b/A1_Experiment_Sheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Feature Representation</t>
   </si>
@@ -67,10 +67,13 @@
     <t>DecisionTreeClassifier</t>
   </si>
   <si>
+    <t>criterion=gini</t>
+  </si>
+  <si>
     <t>SVMClassifier</t>
   </si>
   <si>
-    <t/>
+    <t>C=1.0</t>
   </si>
 </sst>
 </file>
@@ -103,7 +106,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -155,11 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -167,15 +173,21 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -486,14 +498,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="33.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="30.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="27.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="33.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="30.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="27.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -509,214 +521,246 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>0.4653</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>0.4865</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>0.4653</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="5">
         <v>0.4675</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>0.4653</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>0.4865</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>0.4653</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <v>0.4675</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>0.6</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>0.6034</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <v>0.6</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="5">
         <v>0.5967</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>0.598</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>0.5954</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>0.598</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="5">
         <v>0.5925</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="E6" s="5">
+        <v>0.5485</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.5568</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.5485</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.5494</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="E7" s="5">
+        <v>0.5446</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.5499</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.5446</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.5445</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="E8" s="5">
+        <v>0.6376</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.6522</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.6376</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.6058</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="E9" s="5">
+        <v>0.6653</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.6707</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.6653</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.6588</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>